<commit_message>
Changed Begin.vi to match spreadsheet. Fixed spreadsheet (talon now jag)
</commit_message>
<xml_diff>
--- a/Documents/Pin Numbers 02-19-13.xlsx
+++ b/Documents/Pin Numbers 02-19-13.xlsx
@@ -162,7 +162,7 @@
     <t>Digital IO Channel     2</t>
   </si>
   <si>
-    <t>Shooter Angle Tallon</t>
+    <t>Shooter Angle Jagguar</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>